<commit_message>
simplify Romanian residential and commercial building classes (following local expert feedback)
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Romania_COM.xlsx
+++ b/com_mapping_schemes/mapping_Romania_COM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFC1F4-12F0-6C4E-9DE0-4FB616797283}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18900" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -57,7 +63,7 @@
 1.5% CR/LFM+CDL/HBET:6-/Offices
 4.5% CR/LFM+CDM/H:2/Offices
 3.0% CR/LFM+CDM/HBET:6-/Offices
-0.0% ER+ETC/LWAL+CDN/H:1/Offices
+0.0% MUR+ADO/LWAL+CDN/H:1/Offices
 0.0% MCF/LWAL+CDL/H:1/Offices
 0.0% MCF/LWAL+CDN/H:1/Offices
 0.0% MCF/LWAL+CDN/H:2/Offices</t>
@@ -95,7 +101,7 @@
 0.0% CR/LFM+CDL/HBET:6-/Trade
 0.0% CR/LFM+CDM/H:2/Trade
 0.0% CR/LFM+CDM/HBET:6-/Trade
-18.0% ER+ETC/LWAL+CDN/H:1/Trade
+18.0% MUR+ADO/LWAL+CDN/H:1/Trade
 20.0% MCF/LWAL+CDL/H:1/Trade
 20.0% MCF/LWAL+CDN/H:1/Trade
 10.0% MCF/LWAL+CDN/H:2/Trade</t>
@@ -133,7 +139,7 @@
  1.5% CR/LFM+CDL/HBET:6-/Hotels
  4.5% CR/LFM+CDM/H:2/Hotels
  3.0% CR/LFM+CDM/HBET:6-/Hotels
- 0.0% ER+ETC/LWAL+CDN/H:1/Hotels
+ 0.0% MUR+ADO/LWAL+CDN/H:1/Hotels
  0.0% MCF/LWAL+CDL/H:1/Hotels
  0.0% MCF/LWAL+CDN/H:1/Hotels
  0.0% MCF/LWAL+CDN/H:2/Hotels</t>
@@ -142,8 +148,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,10 +201,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -206,6 +215,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -252,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,9 +301,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,6 +353,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +546,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,14 +571,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update mapping scheme for commercial for Romania (replace CR/LFM with CR/LFINF, as per residential)
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Romania_COM.xlsx
+++ b/com_mapping_schemes/mapping_Romania_COM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFC1F4-12F0-6C4E-9DE0-4FB616797283}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3BF871-74CC-F949-9C4A-823BE44C8510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18900" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21300" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
@@ -54,15 +54,15 @@
 0.5% CR/LFINF+CDN/H:2/Offices
 1.0% CR/LFINF+CDN/HBET:3-5/Offices
 0.5% CR/LFINF+CDN/HBET:6-/Offices
-5.0% CR/LFM+CDM/HBET:3-5/Offices
-3.5% CR/LFM+CDH/H:2/Offices
-7.0% CR/LFM+CDH/HBET:3-5/Offices
-3.0% CR/LFM+CDH/HBET:6-/Offices
-2.0% CR/LFM+CDL/H:2/Offices
-3.5% CR/LFM+CDL/HBET:3-5/Offices
-1.5% CR/LFM+CDL/HBET:6-/Offices
-4.5% CR/LFM+CDM/H:2/Offices
-3.0% CR/LFM+CDM/HBET:6-/Offices
+5.0% CR/LFINF+CDM/HBET:3-5/Offices
+3.5% CR/LFINF+CDH/H:2/Offices
+7.0% CR/LFINF+CDH/HBET:3-5/Offices
+3.0% CR/LFINF+CDH/HBET:6-/Offices
+2.0% CR/LFINF+CDL/H:2/Offices
+3.5% CR/LFINF+CDL/HBET:3-5/Offices
+1.5% CR/LFINF+CDL/HBET:6-/Offices
+4.5% CR/LFINF+CDM/H:2/Offices
+3.0% CR/LFINF+CDM/HBET:6-/Offices
 0.0% MUR+ADO/LWAL+CDN/H:1/Offices
 0.0% MCF/LWAL+CDL/H:1/Offices
 0.0% MCF/LWAL+CDN/H:1/Offices
@@ -92,15 +92,15 @@
 0.5% CR/LFINF+CDN/H:2/Trade
 0.5% CR/LFINF+CDN/HBET:3-5/Trade
 0.0% CR/LFINF+CDN/HBET:6-/Trade
-0.0% CR/LFM+CDM/HBET:3-5/Trade
-0.0% CR/LFM+CDH/H:2/Trade
-0.0% CR/LFM+CDH/HBET:3-5/Trade
-0.0% CR/LFM+CDH/HBET:6-/Trade
-0.0% CR/LFM+CDL/H:2/Trade
-0.0% CR/LFM+CDL/HBET:3-5/Trade
-0.0% CR/LFM+CDL/HBET:6-/Trade
-0.0% CR/LFM+CDM/H:2/Trade
-0.0% CR/LFM+CDM/HBET:6-/Trade
+0.0% CR/LFINF+CDM/HBET:3-5/Trade
+0.0% CR/LFINF+CDH/H:2/Trade
+0.0% CR/LFINF+CDH/HBET:3-5/Trade
+0.0% CR/LFINF+CDH/HBET:6-/Trade
+0.0% CR/LFINF+CDL/H:2/Trade
+0.0% CR/LFINF+CDL/HBET:3-5/Trade
+0.0% CR/LFINF+CDL/HBET:6-/Trade
+0.0% CR/LFINF+CDM/H:2/Trade
+0.0% CR/LFINF+CDM/HBET:6-/Trade
 18.0% MUR+ADO/LWAL+CDN/H:1/Trade
 20.0% MCF/LWAL+CDL/H:1/Trade
 20.0% MCF/LWAL+CDN/H:1/Trade
@@ -130,15 +130,15 @@
  0.5% CR/LFINF+CDN/H:2/Hotels
  1.0% CR/LFINF+CDN/HBET:3-5/Hotels
  0.5% CR/LFINF+CDN/HBET:6-/Hotels
- 5.0% CR/LFM+CDM/HBET:3-5/Hotels
- 3.5% CR/LFM+CDH/H:2/Hotels
- 7.0% CR/LFM+CDH/HBET:3-5/Hotels
- 3.0% CR/LFM+CDH/HBET:6-/Hotels
- 2.0% CR/LFM+CDL/H:2/Hotels
- 3.5% CR/LFM+CDL/HBET:3-5/Hotels
- 1.5% CR/LFM+CDL/HBET:6-/Hotels
- 4.5% CR/LFM+CDM/H:2/Hotels
- 3.0% CR/LFM+CDM/HBET:6-/Hotels
+ 5.0% CR/LFINF+CDM/HBET:3-5/Hotels
+ 3.5% CR/LFINF+CDH/H:2/Hotels
+ 7.0% CR/LFINF+CDH/HBET:3-5/Hotels
+ 3.0% CR/LFINF+CDH/HBET:6-/Hotels
+ 2.0% CR/LFINF+CDL/H:2/Hotels
+ 3.5% CR/LFINF+CDL/HBET:3-5/Hotels
+ 1.5% CR/LFINF+CDL/HBET:6-/Hotels
+ 4.5% CR/LFINF+CDM/H:2/Hotels
+ 3.0% CR/LFINF+CDM/HBET:6-/Hotels
  0.0% MUR+ADO/LWAL+CDN/H:1/Hotels
  0.0% MCF/LWAL+CDL/H:1/Hotels
  0.0% MCF/LWAL+CDN/H:1/Hotels
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reduce adobe and increase confined masonry in trade building distribution (commercial)
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Romania_COM.xlsx
+++ b/com_mapping_schemes/mapping_Romania_COM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3BF871-74CC-F949-9C4A-823BE44C8510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B173D38-A9F7-1345-8A53-7A4ADE6FA2AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="21300" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,44 +69,6 @@
 0.0% MCF/LWAL+CDN/H:2/Offices</t>
   </si>
   <si>
-    <t>2.0% CR+PC/LWAL+CDL/H:1/Trade
-2.0% CR+PC/LWAL+CDL/H:2/Trade
-0.0% CR+PC/LWAL+CDL/HBET:3-5/Trade
-0.0% CR+PC/LWAL+CDL/HBET:6-/Trade
-5.0% CR+PC/LWAL+CDM/H:1/Trade
-5.0% CR+PC/LWAL+CDM/H:2/Trade
-0.0% CR+PC/LWAL+CDM/HBET:3-5/Trade
-0.0% CR+PC/LWAL+CDM/HBET:6-/Trade
-3.5% CR/LFINF+CDH/H:1/Trade
-3.5% CR/LFINF+CDH/H:2/Trade
-0.0% CR/LFINF+CDH/HBET:3-5/Trade
-0.0% CR/LFINF+CDH/HBET:6-/Trade
-2.0% CR/LFINF+CDL/H:1/Trade
-1.5% CR/LFINF+CDL/H:2/Trade
-0.0% CR/LFINF+CDL/HBET:3-5/Trade
-3.0% CR/LFINF+CDM/H:1/Trade
-3.0% CR/LFINF+CDM/H:2/Trade
-0.0% CR/LFINF+CDM/HBET:3-5/Trade
-0.0% CR/LFINF+CDM/HBET:6-/Trade
-0.5% CR/LFINF+CDN/H:1/Trade
-0.5% CR/LFINF+CDN/H:2/Trade
-0.5% CR/LFINF+CDN/HBET:3-5/Trade
-0.0% CR/LFINF+CDN/HBET:6-/Trade
-0.0% CR/LFINF+CDM/HBET:3-5/Trade
-0.0% CR/LFINF+CDH/H:2/Trade
-0.0% CR/LFINF+CDH/HBET:3-5/Trade
-0.0% CR/LFINF+CDH/HBET:6-/Trade
-0.0% CR/LFINF+CDL/H:2/Trade
-0.0% CR/LFINF+CDL/HBET:3-5/Trade
-0.0% CR/LFINF+CDL/HBET:6-/Trade
-0.0% CR/LFINF+CDM/H:2/Trade
-0.0% CR/LFINF+CDM/HBET:6-/Trade
-18.0% MUR+ADO/LWAL+CDN/H:1/Trade
-20.0% MCF/LWAL+CDL/H:1/Trade
-20.0% MCF/LWAL+CDN/H:1/Trade
-10.0% MCF/LWAL+CDN/H:2/Trade</t>
-  </si>
-  <si>
     <t>0.0% CR+PC/LWAL+CDL/H:1/Hotels
  2.0% CR+PC/LWAL+CDL/H:2/Hotels
  3.0% CR+PC/LWAL+CDL/HBET:3-5/Hotels
@@ -143,6 +105,44 @@
  0.0% MCF/LWAL+CDL/H:1/Hotels
  0.0% MCF/LWAL+CDN/H:1/Hotels
  0.0% MCF/LWAL+CDN/H:2/Hotels</t>
+  </si>
+  <si>
+    <t>2.0% CR+PC/LWAL+CDL/H:1/Trade
+2.0% CR+PC/LWAL+CDL/H:2/Trade
+0.0% CR+PC/LWAL+CDL/HBET:3-5/Trade
+0.0% CR+PC/LWAL+CDL/HBET:6-/Trade
+5.0% CR+PC/LWAL+CDM/H:1/Trade
+5.0% CR+PC/LWAL+CDM/H:2/Trade
+0.0% CR+PC/LWAL+CDM/HBET:3-5/Trade
+0.0% CR+PC/LWAL+CDM/HBET:6-/Trade
+3.5% CR/LFINF+CDH/H:1/Trade
+3.5% CR/LFINF+CDH/H:2/Trade
+0.0% CR/LFINF+CDH/HBET:3-5/Trade
+0.0% CR/LFINF+CDH/HBET:6-/Trade
+2.0% CR/LFINF+CDL/H:1/Trade
+1.5% CR/LFINF+CDL/H:2/Trade
+0.0% CR/LFINF+CDL/HBET:3-5/Trade
+3.0% CR/LFINF+CDM/H:1/Trade
+3.0% CR/LFINF+CDM/H:2/Trade
+0.0% CR/LFINF+CDM/HBET:3-5/Trade
+0.0% CR/LFINF+CDM/HBET:6-/Trade
+0.5% CR/LFINF+CDN/H:1/Trade
+0.5% CR/LFINF+CDN/H:2/Trade
+0.5% CR/LFINF+CDN/HBET:3-5/Trade
+0.0% CR/LFINF+CDN/HBET:6-/Trade
+0.0% CR/LFINF+CDM/HBET:3-5/Trade
+0.0% CR/LFINF+CDH/H:2/Trade
+0.0% CR/LFINF+CDH/HBET:3-5/Trade
+0.0% CR/LFINF+CDH/HBET:6-/Trade
+0.0% CR/LFINF+CDL/H:2/Trade
+0.0% CR/LFINF+CDL/HBET:3-5/Trade
+0.0% CR/LFINF+CDL/HBET:6-/Trade
+0.0% CR/LFINF+CDM/H:2/Trade
+0.0% CR/LFINF+CDM/HBET:6-/Trade
+8.0% MUR+ADO/LWAL+CDN/H:1/Trade
+25.0% MCF/LWAL+CDL/H:1/Trade
+25.0% MCF/LWAL+CDN/H:1/Trade
+10.0% MCF/LWAL+CDN/H:2/Trade</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -576,10 +576,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>